<commit_message>
Update 33 ohm resistor
</commit_message>
<xml_diff>
--- a/BOM_nextPCB(serviA2).xlsx
+++ b/BOM_nextPCB(serviA2).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://helbe-my.sharepoint.com/personal/sylvain_dewez_student_hel_be/Documents/BAC 3/Stage/Déroulement/fichiers/Github/MICHA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1205" documentId="11_AD4D9D64A577C15A4A5418E8A0DB70CC5BDEDD83" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{5A29CB97-55B2-474C-B990-FC3D8A2538DC}"/>
+  <xr:revisionPtr revIDLastSave="1210" documentId="11_AD4D9D64A577C15A4A5418E8A0DB70CC5BDEDD83" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C4D4780A-8B29-4783-AB3B-EE0FAB4BE2C3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="2550" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V4.0" sheetId="3" r:id="rId1"/>
@@ -602,12 +602,6 @@
     <t>https://www.mouser.be/ProductDetail/Phoenix-Contact/1725656?qs=%2Fha2pyFaduisMLVvmyA1Rh0mEWT0DKYxlzilMJiDQbY%3D</t>
   </si>
   <si>
-    <t>https://www.mouser.be/ProductDetail/Yageo/RT1206BRD0733RL?qs=sGAEpiMZZMvdGkrng054t%252BSYh%252B1gqt95ZImaTMtcXyM%3D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RT1206BRD0733RL </t>
-  </si>
-  <si>
     <t>Pullup optocoupleur</t>
   </si>
   <si>
@@ -639,6 +633,12 @@
   </si>
   <si>
     <t>https://www.mouser.be/ProductDetail/Diodes-Incorporated/SDM10M45SD-7-F?qs=%2Fha2pyFadujjRkPixxzQ28uXDzT00Y%252Bd3v2piDiuOZ%252BOgoOZIcgrJQ%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/Panasonic/ERJ-P08D33R0V?qs=sGAEpiMZZMvdGkrng054t5hHekyimr99UaPO9LKWRes%3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERJ-P08D33R0V </t>
   </si>
 </sst>
 </file>
@@ -1523,8 +1523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00C6BB1E-CDC9-41D8-A56D-50F2079A148E}">
   <dimension ref="A1:T64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1735,22 +1735,22 @@
         <v>4</v>
       </c>
       <c r="B9" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>195</v>
-      </c>
-      <c r="C9" s="23" t="s">
-        <v>196</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>197</v>
       </c>
       <c r="E9" s="8">
         <v>4</v>
       </c>
       <c r="F9" s="24" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="H9" s="53">
         <f>[1]Feuil1!$F$24</f>
@@ -1758,7 +1758,7 @@
       </c>
       <c r="I9" s="25"/>
       <c r="J9" s="10" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="K9" s="11"/>
       <c r="L9" s="11"/>
@@ -2038,7 +2038,7 @@
         <v>1</v>
       </c>
       <c r="F16" s="34" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G16" s="18" t="s">
         <v>11</v>
@@ -2048,10 +2048,10 @@
         <v>0</v>
       </c>
       <c r="I16" s="35" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="J16" s="36" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="K16" s="37"/>
       <c r="L16" s="37"/>
@@ -2303,7 +2303,7 @@
         <v>6</v>
       </c>
       <c r="F24" s="24" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="G24" s="8" t="s">
         <v>11</v>
@@ -2316,7 +2316,7 @@
         <v>176</v>
       </c>
       <c r="J24" s="10" t="s">
-        <v>188</v>
+        <v>199</v>
       </c>
       <c r="K24" s="11"/>
       <c r="L24" s="11"/>
@@ -2444,7 +2444,7 @@
         <v>3</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G28" s="13" t="s">
         <v>173</v>
@@ -2797,7 +2797,7 @@
         <v>26</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C38" s="18" t="s">
         <v>102</v>

</xml_diff>

<commit_message>
Components for MICHA v2 added
</commit_message>
<xml_diff>
--- a/BOM_nextPCB(serviA2).xlsx
+++ b/BOM_nextPCB(serviA2).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://helbe-my.sharepoint.com/personal/sylvain_dewez_student_hel_be/Documents/BAC 3/Stage/Déroulement/fichiers/Github/MICHA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1210" documentId="11_AD4D9D64A577C15A4A5418E8A0DB70CC5BDEDD83" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C4D4780A-8B29-4783-AB3B-EE0FAB4BE2C3}"/>
+  <xr:revisionPtr revIDLastSave="1226" documentId="11_AD4D9D64A577C15A4A5418E8A0DB70CC5BDEDD83" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{464EF9F3-FFD0-4022-BBC5-D89AF3DBEDE5}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="2550" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V4.0" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="209">
   <si>
     <t>Item</t>
   </si>
@@ -639,6 +639,30 @@
   </si>
   <si>
     <t xml:space="preserve">ERJ-P08D33R0V </t>
+  </si>
+  <si>
+    <t>Bouton poussoir à Led rouge 12V</t>
+  </si>
+  <si>
+    <t>Bouton poussoir à Led jaune 12V</t>
+  </si>
+  <si>
+    <t>rouge, off - (on)</t>
+  </si>
+  <si>
+    <t>vert, off - (on)</t>
+  </si>
+  <si>
+    <t>jaune, off - (on)</t>
+  </si>
+  <si>
+    <t>LP10A1AY</t>
+  </si>
+  <si>
+    <t>LP10A1AR</t>
+  </si>
+  <si>
+    <t>LP10A1AG</t>
   </si>
 </sst>
 </file>
@@ -816,7 +840,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -1008,7 +1032,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1053,6 +1076,10 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -1060,13 +1087,48 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1149,7 +1211,7 @@
         </row>
         <row r="12">
           <cell r="F12">
-            <v>0</v>
+            <v>100</v>
           </cell>
         </row>
         <row r="13">
@@ -1159,7 +1221,7 @@
         </row>
         <row r="15">
           <cell r="F15">
-            <v>0</v>
+            <v>16</v>
           </cell>
         </row>
         <row r="16">
@@ -1169,7 +1231,7 @@
         </row>
         <row r="17">
           <cell r="F17">
-            <v>0</v>
+            <v>4</v>
           </cell>
         </row>
         <row r="19">
@@ -1189,7 +1251,7 @@
         </row>
         <row r="24">
           <cell r="F24">
-            <v>0</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="25">
@@ -1214,7 +1276,7 @@
         </row>
         <row r="32">
           <cell r="F32">
-            <v>0</v>
+            <v>10</v>
           </cell>
         </row>
         <row r="33">
@@ -1234,7 +1296,7 @@
         </row>
         <row r="38">
           <cell r="F38">
-            <v>0</v>
+            <v>5</v>
           </cell>
         </row>
         <row r="39">
@@ -1244,12 +1306,27 @@
         </row>
         <row r="40">
           <cell r="F40">
-            <v>1</v>
+            <v>2</v>
           </cell>
         </row>
         <row r="41">
           <cell r="F41">
-            <v>0</v>
+            <v>4</v>
+          </cell>
+        </row>
+        <row r="42">
+          <cell r="F42">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="F43">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="F44">
+            <v>2</v>
           </cell>
         </row>
       </sheetData>
@@ -1523,8 +1600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00C6BB1E-CDC9-41D8-A56D-50F2079A148E}">
   <dimension ref="A1:T64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1536,7 +1613,7 @@
     <col min="5" max="5" width="4.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.7109375" style="51" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" style="58" customWidth="1"/>
     <col min="9" max="9" width="39.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="11.42578125" style="1"/>
   </cols>
@@ -1571,7 +1648,7 @@
       <c r="G4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="52" t="s">
+      <c r="H4" s="51" t="s">
         <v>156</v>
       </c>
       <c r="I4" s="5" t="s">
@@ -1613,7 +1690,7 @@
       <c r="G5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="53" t="str">
+      <c r="H5" s="52" t="str">
         <f>[1]Feuil1!$F$2</f>
         <v>&gt;20</v>
       </c>
@@ -1654,7 +1731,7 @@
       <c r="G6" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="54" t="str">
+      <c r="H6" s="53" t="str">
         <f>[1]Feuil1!$F$3</f>
         <v>&gt;20</v>
       </c>
@@ -1695,7 +1772,7 @@
       <c r="G7" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="55" t="str">
+      <c r="H7" s="54" t="str">
         <f>[1]Feuil1!$F$4</f>
         <v>&gt;20</v>
       </c>
@@ -1714,7 +1791,7 @@
         <v>151</v>
       </c>
       <c r="G8" s="8"/>
-      <c r="H8" s="53"/>
+      <c r="H8" s="52"/>
       <c r="I8" s="25"/>
       <c r="J8" s="10" t="s">
         <v>152</v>
@@ -1731,7 +1808,7 @@
       <c r="T8" s="11"/>
     </row>
     <row r="9" spans="1:20" ht="13.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="63">
+      <c r="A9" s="62">
         <v>4</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -1752,9 +1829,9 @@
       <c r="G9" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="H9" s="53">
+      <c r="H9" s="52">
         <f>[1]Feuil1!$F$24</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I9" s="25"/>
       <c r="J9" s="10" t="s">
@@ -1793,7 +1870,7 @@
       <c r="G10" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="54">
+      <c r="H10" s="53">
         <f>[1]Feuil1!$F$28</f>
         <v>1</v>
       </c>
@@ -1836,9 +1913,9 @@
       <c r="G11" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="H11" s="54">
+      <c r="H11" s="53">
         <f>[1]Feuil1!$F$38</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I11" s="31" t="s">
         <v>31</v>
@@ -1879,7 +1956,7 @@
       <c r="G12" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="H12" s="54">
+      <c r="H12" s="53">
         <f>[1]Feuil1!$F$5</f>
         <v>4</v>
       </c>
@@ -1918,7 +1995,7 @@
       <c r="G13" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="H13" s="54">
+      <c r="H13" s="53">
         <f>[1]Feuil1!$F$36</f>
         <v>18</v>
       </c>
@@ -1959,7 +2036,7 @@
       <c r="G14" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="H14" s="54" t="str">
+      <c r="H14" s="53" t="str">
         <f>[1]Feuil1!$F$6</f>
         <v>&gt;20</v>
       </c>
@@ -2002,7 +2079,7 @@
       <c r="G15" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="H15" s="56">
+      <c r="H15" s="55">
         <f>[1]Feuil1!$F$11</f>
         <v>0</v>
       </c>
@@ -2043,9 +2120,9 @@
       <c r="G16" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="H16" s="57">
+      <c r="H16" s="56">
         <f>[1]Feuil1!$F$12</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="I16" s="35" t="s">
         <v>188</v>
@@ -2072,7 +2149,7 @@
       <c r="E17" s="8"/>
       <c r="F17" s="9"/>
       <c r="G17" s="39"/>
-      <c r="H17" s="58"/>
+      <c r="H17" s="57"/>
       <c r="I17" s="25"/>
       <c r="J17" s="40"/>
       <c r="K17" s="27"/>
@@ -2108,7 +2185,7 @@
       <c r="G18" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="H18" s="55" t="str">
+      <c r="H18" s="54" t="str">
         <f>[1]Feuil1!$F$8</f>
         <v>&gt;20</v>
       </c>
@@ -2129,7 +2206,7 @@
         <v>149</v>
       </c>
       <c r="G19" s="8"/>
-      <c r="H19" s="53"/>
+      <c r="H19" s="52"/>
       <c r="I19" s="25"/>
       <c r="J19" s="10" t="s">
         <v>150</v>
@@ -2167,7 +2244,7 @@
       <c r="G20" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="54" t="str">
+      <c r="H20" s="53" t="str">
         <f>[1]Feuil1!$F$9</f>
         <v>&gt;20</v>
       </c>
@@ -2210,7 +2287,7 @@
       <c r="G21" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="H21" s="55" t="str">
+      <c r="H21" s="54" t="str">
         <f>[1]Feuil1!$F$10</f>
         <v>&gt;20</v>
       </c>
@@ -2229,7 +2306,7 @@
         <v>147</v>
       </c>
       <c r="G22" s="8"/>
-      <c r="H22" s="53"/>
+      <c r="H22" s="52"/>
       <c r="I22" s="25"/>
       <c r="J22" s="10" t="s">
         <v>148</v>
@@ -2267,7 +2344,7 @@
       <c r="G23" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="H23" s="54">
+      <c r="H23" s="53">
         <f>[1]Feuil1!$F$13</f>
         <v>9</v>
       </c>
@@ -2308,11 +2385,11 @@
       <c r="G24" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H24" s="53">
+      <c r="H24" s="52">
         <f>[1]Feuil1!$F$15</f>
-        <v>0</v>
-      </c>
-      <c r="I24" s="60" t="s">
+        <v>16</v>
+      </c>
+      <c r="I24" s="59" t="s">
         <v>176</v>
       </c>
       <c r="J24" s="10" t="s">
@@ -2349,7 +2426,7 @@
       <c r="G25" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="H25" s="55">
+      <c r="H25" s="54">
         <f>[1]Feuil1!$F$16</f>
         <v>23</v>
       </c>
@@ -2370,7 +2447,7 @@
         <v>119</v>
       </c>
       <c r="G26" s="8"/>
-      <c r="H26" s="53"/>
+      <c r="H26" s="52"/>
       <c r="I26" s="25"/>
       <c r="J26" s="10" t="s">
         <v>146</v>
@@ -2406,11 +2483,11 @@
       <c r="G27" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H27" s="54">
+      <c r="H27" s="53">
         <f>[1]Feuil1!$F$33</f>
         <v>6</v>
       </c>
-      <c r="I27" s="61" t="s">
+      <c r="I27" s="60" t="s">
         <v>76</v>
       </c>
       <c r="J27" s="16" t="s">
@@ -2449,11 +2526,11 @@
       <c r="G28" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="H28" s="54">
+      <c r="H28" s="53">
         <f>[1]Feuil1!$F$32</f>
-        <v>0</v>
-      </c>
-      <c r="I28" s="61" t="s">
+        <v>10</v>
+      </c>
+      <c r="I28" s="60" t="s">
         <v>174</v>
       </c>
       <c r="J28" s="16" t="s">
@@ -2490,11 +2567,11 @@
       <c r="G29" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="H29" s="54">
+      <c r="H29" s="53">
         <f>[1]Feuil1!$F$39</f>
         <v>1</v>
       </c>
-      <c r="I29" s="61"/>
+      <c r="I29" s="60"/>
       <c r="J29" s="16"/>
       <c r="K29" s="17"/>
       <c r="L29" s="17"/>
@@ -2527,11 +2604,11 @@
       <c r="G30" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="H30" s="54">
+      <c r="H30" s="53">
         <f>[1]Feuil1!$F$40</f>
-        <v>1</v>
-      </c>
-      <c r="I30" s="61"/>
+        <v>2</v>
+      </c>
+      <c r="I30" s="60"/>
       <c r="J30" s="31" t="s">
         <v>37</v>
       </c>
@@ -2568,11 +2645,11 @@
       <c r="G31" s="13" t="s">
         <v>181</v>
       </c>
-      <c r="H31" s="54">
+      <c r="H31" s="53">
         <f>[1]Feuil1!$F$41</f>
-        <v>0</v>
-      </c>
-      <c r="I31" s="61"/>
+        <v>4</v>
+      </c>
+      <c r="I31" s="60"/>
       <c r="J31" s="31" t="s">
         <v>179</v>
       </c>
@@ -2609,11 +2686,11 @@
       <c r="G32" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="H32" s="54">
+      <c r="H32" s="53">
         <f>[1]Feuil1!$F$37</f>
         <v>6</v>
       </c>
-      <c r="I32" s="61" t="s">
+      <c r="I32" s="60" t="s">
         <v>78</v>
       </c>
       <c r="J32" s="16" t="s">
@@ -2652,7 +2729,7 @@
       <c r="G33" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="H33" s="55">
+      <c r="H33" s="54">
         <v>18</v>
       </c>
       <c r="I33" s="21" t="s">
@@ -2674,7 +2751,7 @@
         <v>141</v>
       </c>
       <c r="G34" s="8"/>
-      <c r="H34" s="53"/>
+      <c r="H34" s="52"/>
       <c r="I34" s="25"/>
       <c r="J34" s="10" t="s">
         <v>140</v>
@@ -2694,7 +2771,7 @@
       <c r="A35" s="45">
         <v>24</v>
       </c>
-      <c r="B35" s="62" t="s">
+      <c r="B35" s="61" t="s">
         <v>184</v>
       </c>
       <c r="C35" s="13" t="s">
@@ -2712,9 +2789,9 @@
       <c r="G35" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="H35" s="54">
+      <c r="H35" s="53">
         <f>[1]Feuil1!$F$17</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I35" s="31" t="s">
         <v>186</v>
@@ -2755,7 +2832,7 @@
       <c r="G36" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="H36" s="55">
+      <c r="H36" s="54">
         <f>[1]Feuil1!$F$30</f>
         <v>6</v>
       </c>
@@ -2776,7 +2853,7 @@
         <v>104</v>
       </c>
       <c r="G37" s="8"/>
-      <c r="H37" s="53"/>
+      <c r="H37" s="52"/>
       <c r="I37" s="25"/>
       <c r="J37" s="10" t="s">
         <v>137</v>
@@ -2814,7 +2891,7 @@
       <c r="G38" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="H38" s="55">
+      <c r="H38" s="54">
         <f>[1]Feuil1!$F$20</f>
         <v>17</v>
       </c>
@@ -2835,7 +2912,7 @@
         <v>117</v>
       </c>
       <c r="G39" s="8"/>
-      <c r="H39" s="53"/>
+      <c r="H39" s="52"/>
       <c r="I39" s="25"/>
       <c r="J39" s="10" t="s">
         <v>136</v>
@@ -2871,7 +2948,7 @@
       <c r="G40" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="H40" s="54">
+      <c r="H40" s="53">
         <f>[1]Feuil1!$F$19</f>
         <v>0</v>
       </c>
@@ -2912,7 +2989,7 @@
       <c r="G41" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="H41" s="55">
+      <c r="H41" s="54">
         <f>[1]Feuil1!$F$21</f>
         <v>5</v>
       </c>
@@ -2933,7 +3010,7 @@
         <v>142</v>
       </c>
       <c r="G42" s="8"/>
-      <c r="H42" s="53"/>
+      <c r="H42" s="52"/>
       <c r="I42" s="25"/>
       <c r="J42" s="10" t="s">
         <v>143</v>
@@ -2969,7 +3046,7 @@
       <c r="G43" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="H43" s="55">
+      <c r="H43" s="54">
         <f>[1]Feuil1!$F$25</f>
         <v>6</v>
       </c>
@@ -2990,7 +3067,7 @@
         <v>144</v>
       </c>
       <c r="G44" s="8"/>
-      <c r="H44" s="53"/>
+      <c r="H44" s="52"/>
       <c r="I44" s="25"/>
       <c r="J44" s="10" t="s">
         <v>145</v>
@@ -3024,7 +3101,7 @@
       <c r="G45" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="H45" s="54">
+      <c r="H45" s="53">
         <f>[1]Feuil1!$F$26</f>
         <v>3</v>
       </c>
@@ -3043,109 +3120,144 @@
       <c r="S45" s="17"/>
       <c r="T45" s="17"/>
     </row>
-    <row r="46" spans="1:20" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="45">
+    <row r="46" spans="1:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="12">
         <v>31</v>
       </c>
-      <c r="B46" s="18"/>
-      <c r="C46" s="18" t="s">
+      <c r="B46" s="17"/>
+      <c r="C46" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="D46" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="E46" s="18">
+      <c r="D46" s="67" t="s">
+        <v>203</v>
+      </c>
+      <c r="E46" s="67">
         <v>1</v>
       </c>
-      <c r="F46" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="G46" s="18" t="s">
+      <c r="F46" s="67" t="s">
+        <v>207</v>
+      </c>
+      <c r="G46" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="H46" s="55"/>
-      <c r="I46" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="J46" s="22" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A47" s="45">
+      <c r="H46" s="68">
+        <f>[1]Feuil1!$F$42</f>
+        <v>2</v>
+      </c>
+      <c r="I46" s="17"/>
+      <c r="J46" s="17"/>
+      <c r="K46" s="17"/>
+      <c r="L46" s="17"/>
+      <c r="M46" s="17"/>
+      <c r="N46" s="17"/>
+      <c r="O46" s="17"/>
+      <c r="P46" s="17"/>
+      <c r="Q46" s="17"/>
+      <c r="R46" s="17"/>
+      <c r="S46" s="17"/>
+      <c r="T46" s="17"/>
+    </row>
+    <row r="47" spans="1:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="12">
         <v>32</v>
       </c>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18" t="s">
+      <c r="B47" s="17"/>
+      <c r="C47" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="D47" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="E47" s="18">
+      <c r="D47" s="67" t="s">
+        <v>204</v>
+      </c>
+      <c r="E47" s="67">
         <v>1</v>
       </c>
-      <c r="F47" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="G47" s="18" t="s">
+      <c r="F47" s="67" t="s">
+        <v>208</v>
+      </c>
+      <c r="G47" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="H47" s="55"/>
-      <c r="I47" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="J47" s="22" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A48" s="45">
+      <c r="H47" s="68">
+        <f>[1]Feuil1!$F$43</f>
+        <v>2</v>
+      </c>
+      <c r="I47" s="17"/>
+      <c r="J47" s="17"/>
+      <c r="K47" s="17"/>
+      <c r="L47" s="17"/>
+      <c r="M47" s="17"/>
+      <c r="N47" s="17"/>
+      <c r="O47" s="17"/>
+      <c r="P47" s="17"/>
+      <c r="Q47" s="17"/>
+      <c r="R47" s="17"/>
+      <c r="S47" s="17"/>
+      <c r="T47" s="17"/>
+    </row>
+    <row r="48" spans="1:20" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="12">
         <v>33</v>
       </c>
-      <c r="B48" s="18"/>
-      <c r="C48" s="18" t="s">
+      <c r="B48" s="17"/>
+      <c r="C48" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="D48" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="E48" s="18">
+      <c r="D48" s="67" t="s">
+        <v>205</v>
+      </c>
+      <c r="E48" s="67">
         <v>1</v>
       </c>
-      <c r="F48" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="G48" s="18" t="s">
+      <c r="F48" s="67" t="s">
+        <v>206</v>
+      </c>
+      <c r="G48" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="H48" s="55"/>
-      <c r="I48" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="J48" s="22" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="45">
+      <c r="H48" s="68">
+        <f>[1]Feuil1!$F$44</f>
+        <v>2</v>
+      </c>
+      <c r="I48" s="17"/>
+      <c r="J48" s="17"/>
+      <c r="K48" s="17"/>
+      <c r="L48" s="17"/>
+      <c r="M48" s="17"/>
+      <c r="N48" s="17"/>
+      <c r="O48" s="17"/>
+      <c r="P48" s="17"/>
+      <c r="Q48" s="17"/>
+      <c r="R48" s="17"/>
+      <c r="S48" s="17"/>
+      <c r="T48" s="17"/>
+    </row>
+    <row r="49" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="63">
         <v>34</v>
       </c>
       <c r="B49" s="18"/>
       <c r="C49" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="D49" s="18"/>
+        <v>39</v>
+      </c>
+      <c r="D49" s="18" t="s">
+        <v>89</v>
+      </c>
       <c r="E49" s="18">
         <v>1</v>
       </c>
-      <c r="F49" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="G49" s="18"/>
-      <c r="H49" s="55"/>
-      <c r="I49" s="18"/>
-      <c r="J49" s="22"/>
+      <c r="F49" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="G49" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="H49" s="54"/>
+      <c r="I49" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="J49" s="22" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="45">
@@ -3153,105 +3265,119 @@
       </c>
       <c r="B50" s="18"/>
       <c r="C50" s="18" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="D50" s="18" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="E50" s="18">
-        <v>4</v>
-      </c>
-      <c r="F50" s="18" t="s">
-        <v>22</v>
+        <v>1</v>
+      </c>
+      <c r="F50" s="20" t="s">
+        <v>92</v>
       </c>
       <c r="G50" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="H50" s="55"/>
-      <c r="I50" s="18"/>
-      <c r="J50" s="22"/>
-    </row>
-    <row r="51" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="H50" s="54"/>
+      <c r="I50" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="J50" s="22" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="45">
         <v>36</v>
       </c>
       <c r="B51" s="18"/>
       <c r="C51" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="D51" s="19" t="s">
-        <v>45</v>
+        <v>39</v>
+      </c>
+      <c r="D51" s="18" t="s">
+        <v>154</v>
       </c>
       <c r="E51" s="18">
-        <v>5</v>
-      </c>
-      <c r="F51" s="20"/>
-      <c r="G51" s="18"/>
-      <c r="H51" s="55"/>
-      <c r="I51" s="18"/>
-      <c r="J51" s="22"/>
+        <v>1</v>
+      </c>
+      <c r="F51" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="G51" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="H51" s="54"/>
+      <c r="I51" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="J51" s="22" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="46">
         <v>37</v>
       </c>
-      <c r="B52" s="47"/>
-      <c r="C52" s="47" t="s">
-        <v>47</v>
-      </c>
-      <c r="D52" s="47"/>
-      <c r="E52" s="47">
+      <c r="B52" s="18"/>
+      <c r="C52" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D52" s="18"/>
+      <c r="E52" s="18">
         <v>1</v>
       </c>
-      <c r="F52" s="48"/>
-      <c r="G52" s="47" t="s">
-        <v>48</v>
-      </c>
-      <c r="H52" s="59"/>
-      <c r="I52" s="47"/>
+      <c r="F52" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="G52" s="18"/>
+      <c r="H52" s="54"/>
+      <c r="I52" s="18"/>
       <c r="J52" s="22"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="46">
         <v>38</v>
       </c>
-      <c r="B53" s="47"/>
-      <c r="C53" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="D53" s="47"/>
-      <c r="E53" s="47">
-        <v>3</v>
-      </c>
-      <c r="F53" s="48"/>
-      <c r="G53" s="47" t="s">
-        <v>51</v>
-      </c>
-      <c r="H53" s="59"/>
-      <c r="I53" s="47"/>
+      <c r="B53" s="18"/>
+      <c r="C53" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D53" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="E53" s="18">
+        <v>4</v>
+      </c>
+      <c r="F53" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G53" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="H53" s="54"/>
+      <c r="I53" s="18"/>
       <c r="J53" s="22"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="46">
         <v>39</v>
       </c>
-      <c r="B54" s="47"/>
-      <c r="C54" s="47" t="s">
-        <v>61</v>
-      </c>
-      <c r="D54" s="47"/>
-      <c r="E54" s="47">
-        <v>7</v>
-      </c>
-      <c r="F54" s="48"/>
-      <c r="G54" s="47" t="s">
-        <v>42</v>
-      </c>
-      <c r="H54" s="59"/>
-      <c r="I54" s="47"/>
-      <c r="J54" s="22" t="s">
-        <v>99</v>
-      </c>
+      <c r="B54" s="18"/>
+      <c r="C54" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D54" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="E54" s="18">
+        <v>5</v>
+      </c>
+      <c r="F54" s="20"/>
+      <c r="G54" s="18"/>
+      <c r="H54" s="54"/>
+      <c r="I54" s="18"/>
+      <c r="J54" s="22"/>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="46">
@@ -3259,67 +3385,90 @@
       </c>
       <c r="B55" s="47"/>
       <c r="C55" s="47" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="D55" s="47"/>
       <c r="E55" s="47">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F55" s="48"/>
       <c r="G55" s="47" t="s">
-        <v>42</v>
-      </c>
-      <c r="H55" s="59"/>
+        <v>48</v>
+      </c>
       <c r="I55" s="47"/>
-      <c r="J55" s="22" t="s">
-        <v>100</v>
-      </c>
+      <c r="J55" s="22"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" s="49"/>
+      <c r="A56" s="46">
+        <v>41</v>
+      </c>
       <c r="B56" s="47"/>
-      <c r="C56" s="47"/>
+      <c r="C56" s="47" t="s">
+        <v>50</v>
+      </c>
       <c r="D56" s="47"/>
-      <c r="E56" s="47"/>
-      <c r="F56" s="47"/>
-      <c r="G56" s="47"/>
-      <c r="H56" s="59"/>
+      <c r="E56" s="47">
+        <v>3</v>
+      </c>
+      <c r="F56" s="48"/>
+      <c r="G56" s="47" t="s">
+        <v>51</v>
+      </c>
       <c r="I56" s="47"/>
       <c r="J56" s="22"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" s="49"/>
+      <c r="A57" s="46">
+        <v>42</v>
+      </c>
       <c r="B57" s="47"/>
-      <c r="C57" s="47"/>
+      <c r="C57" s="47" t="s">
+        <v>61</v>
+      </c>
       <c r="D57" s="47"/>
-      <c r="E57" s="47"/>
-      <c r="F57" s="47"/>
-      <c r="G57" s="47"/>
-      <c r="H57" s="59"/>
+      <c r="E57" s="47">
+        <v>7</v>
+      </c>
+      <c r="F57" s="48"/>
+      <c r="G57" s="47" t="s">
+        <v>42</v>
+      </c>
       <c r="I57" s="47"/>
-      <c r="J57" s="22"/>
+      <c r="J57" s="22" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A58" s="49"/>
+      <c r="A58" s="46">
+        <v>43</v>
+      </c>
       <c r="B58" s="47"/>
-      <c r="C58" s="47"/>
+      <c r="C58" s="47" t="s">
+        <v>62</v>
+      </c>
       <c r="D58" s="47"/>
-      <c r="E58" s="47"/>
-      <c r="F58" s="47"/>
-      <c r="G58" s="47"/>
-      <c r="H58" s="59"/>
+      <c r="E58" s="47">
+        <v>7</v>
+      </c>
+      <c r="F58" s="48"/>
+      <c r="G58" s="47" t="s">
+        <v>42</v>
+      </c>
       <c r="I58" s="47"/>
-      <c r="J58" s="22"/>
+      <c r="J58" s="22" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" s="49"/>
+      <c r="A59" s="46">
+        <v>44</v>
+      </c>
       <c r="B59" s="47"/>
       <c r="C59" s="47"/>
       <c r="D59" s="47"/>
       <c r="E59" s="47"/>
       <c r="F59" s="47"/>
       <c r="G59" s="47"/>
-      <c r="H59" s="59"/>
       <c r="I59" s="47"/>
       <c r="J59" s="22"/>
     </row>
@@ -3331,7 +3480,6 @@
       <c r="E60" s="47"/>
       <c r="F60" s="47"/>
       <c r="G60" s="47"/>
-      <c r="H60" s="59"/>
       <c r="I60" s="47"/>
       <c r="J60" s="22"/>
     </row>
@@ -3354,11 +3502,11 @@
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="A16:A17"/>
   </mergeCells>
-  <conditionalFormatting sqref="A5:T45">
-    <cfRule type="expression" dxfId="1" priority="1">
+  <conditionalFormatting sqref="A5:T48">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>$H5&lt;$E5</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>$H5&gt;=$E5</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3371,9 +3519,9 @@
     <hyperlink ref="J10" r:id="rId6" display="https://befr.rs-online.com/web/p/voltage-references/5343037/?cm_mmc=BE-PLA-DS3A-_-google-_-PLA_BE_FR_Semiconductors_Whoop-_-(BE:Whoop!)+Voltage+References-_-5343037&amp;matchtype=&amp;aud-827186183686:pla-533962920232&amp;gclid=Cj0KCQiAst2BBhDJARIsAGo2ldVAY1WrPDjC8paFXGNZEOmkZQx8TcAHaZFOpla8vljzKIUvydHTWN0aArtkEALw_wcB&amp;gclsrc=aw.ds" xr:uid="{4B66D013-D586-47EE-8D64-26CA00366A1F}"/>
     <hyperlink ref="F40" r:id="rId7" tooltip="MC 1,5/ 4-ST-3,5 1840382; Barrette de pression amovible; 3,5mm; pistes: 4; droit; femelle" display="https://www.tme.eu/fr/details/mc1.5_4-st-3.5/borniers-de-serrage-deconnectables/phoenix-contact/mc-1-5-4-st-3-5-1840382/" xr:uid="{CA613C76-B9F0-4233-86C4-BD3E113E3D81}"/>
     <hyperlink ref="F41" r:id="rId8" tooltip="DS1009-18AT1NX; Support: DIP; PIN: 18; 7,62mm; THT; Trame: 2,54mm" display="https://www.tme.eu/fr/details/icvt-18p/supports-dip-standard/connfly/ds1009-18at1nx/" xr:uid="{95D93535-A405-4289-A585-A00FC5365CAE}"/>
-    <hyperlink ref="F47" r:id="rId9" tooltip="VAQ-9-10-12-R; Commutateur: bouton-poussoir; Pos: 2; SPDT; 10A/250VAC; ON-(ON)" display="https://www.tme.eu/fr/details/vaq-9-10-12-r/commutateurs-standards/highly/" xr:uid="{27067EA1-971F-4DC2-992B-9343F6A6CBB2}"/>
-    <hyperlink ref="F46" r:id="rId10" tooltip="VAQ-9-10-12-G; Commutateur: bouton-poussoir; Pos: 2; SPDT; 10A/250VAC; ON-(ON)" display="https://www.tme.eu/fr/details/vaq-9-10-12-g/commutateurs-standards/highly/" xr:uid="{3D237C8C-FF33-4FBD-9F47-23A5FBAF27E4}"/>
-    <hyperlink ref="F48" r:id="rId11" tooltip="VAQ-9-10-12-Y; Commutateur: bouton-poussoir; Pos: 2; SPDT; 10A/250VAC; ON-(ON)" display="https://www.tme.eu/fr/details/vaq-9-10-12-y/commutateurs-standards/highly/" xr:uid="{CE4B8ED0-965D-4C0E-A322-C5B8602B9323}"/>
+    <hyperlink ref="F50" r:id="rId9" tooltip="VAQ-9-10-12-R; Commutateur: bouton-poussoir; Pos: 2; SPDT; 10A/250VAC; ON-(ON)" display="https://www.tme.eu/fr/details/vaq-9-10-12-r/commutateurs-standards/highly/" xr:uid="{27067EA1-971F-4DC2-992B-9343F6A6CBB2}"/>
+    <hyperlink ref="F49" r:id="rId10" tooltip="VAQ-9-10-12-G; Commutateur: bouton-poussoir; Pos: 2; SPDT; 10A/250VAC; ON-(ON)" display="https://www.tme.eu/fr/details/vaq-9-10-12-g/commutateurs-standards/highly/" xr:uid="{3D237C8C-FF33-4FBD-9F47-23A5FBAF27E4}"/>
+    <hyperlink ref="F51" r:id="rId11" tooltip="VAQ-9-10-12-Y; Commutateur: bouton-poussoir; Pos: 2; SPDT; 10A/250VAC; ON-(ON)" display="https://www.tme.eu/fr/details/vaq-9-10-12-y/commutateurs-standards/highly/" xr:uid="{CE4B8ED0-965D-4C0E-A322-C5B8602B9323}"/>
     <hyperlink ref="F36" r:id="rId12" tooltip="SMAZ5V1-13-F; Diode: Zener; 1W; 5,1V; 196mA; SMD; rouleau,bande; SMA; diode simple" display="https://www.tme.eu/be/fr/details/smaz5v1-13-f/diodes-zener-smd/diodes-incorporated/" xr:uid="{CA0324DD-67DE-4ECD-AB47-263AE86E8EBD}"/>
     <hyperlink ref="F20" r:id="rId13" display="https://befr.rs-online.com/web/p/surface-mount-fixed-resistors/7218093/" xr:uid="{A69B2073-EAD3-4F64-994A-E2F02F998664}"/>
     <hyperlink ref="F38" r:id="rId14" tooltip="1SMA5913BT3G; Diode: Zener; 1,5W; 3,3V; SMD; rouleau,bande; SMA; diode simple" display="https://www.tme.eu/be/fr/details/1sma5913bt3g/diodes-zener-smd/on-semiconductor/" xr:uid="{971C21CD-F9A6-4515-A379-2101CBC403C6}"/>

</xml_diff>